<commit_message>
BUG: load the models with saved features
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,11 @@
           <t>model2</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +491,9 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -504,6 +512,9 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: prediction through own model enabled
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -434,12 +434,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>model2</t>
+          <t>newModel</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>hi</t>
+          <t>newModel2</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LYMC</t>
+          <t>LYMF</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -491,7 +491,7 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="n">
+      <c r="C5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -504,6 +504,9 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +530,9 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -535,6 +541,9 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: training on 0 features no longer allowed
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,16 @@
           <t>newModel2</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sdfcsfs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>adasd</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,6 +491,12 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -507,6 +523,9 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -531,6 +550,9 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: error handling added for missing info file
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>adasd</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>model4</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -510,6 +515,9 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -524,6 +532,9 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: bug fixing sort of
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -1,85 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobre\OneDrive\デスクトップ\Software Engineering\SealsProject\GUI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1A61A7-EDC7-4208-9FF7-E0F3F1ACDC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">MODEL_NAME: </t>
-  </si>
-  <si>
-    <t>defaultModel</t>
-  </si>
-  <si>
-    <t>WBC</t>
-  </si>
-  <si>
-    <t>LYMF</t>
-  </si>
-  <si>
-    <t>RBC</t>
-  </si>
-  <si>
-    <t>HGB</t>
-  </si>
-  <si>
-    <t>MCH</t>
-  </si>
-  <si>
-    <t>MCHC</t>
-  </si>
-  <si>
-    <t>MPV</t>
-  </si>
-  <si>
-    <t>PLT</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>GRAN</t>
-  </si>
-  <si>
-    <t>MID</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -98,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,116 +407,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MODEL_NAME: </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defaultModel</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Species</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WBC</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LYMF</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GRAN</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MID</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RBC</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HGB</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MCH</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MCHC</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MPV</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PLT</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: Removed dumping of sex and species variable
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -471,6 +471,31 @@
           <t>save</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>test.pkl</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>sa</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -510,6 +535,9 @@
       <c r="I4" t="n">
         <v>1</v>
       </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -523,6 +551,9 @@
       <c r="D5" t="n">
         <v>1</v>
       </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -545,6 +576,9 @@
       <c r="J6" t="n">
         <v>1</v>
       </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -561,6 +595,9 @@
       <c r="D7" t="n">
         <v>1</v>
       </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -572,6 +609,9 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: reverted to home button commit
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,10 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -433,132 +434,106 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>newModel</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>newModel2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>sdfcsfs</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>adasd</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>model4</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>save</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>help</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>help</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>test.pkl</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>sa</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>WBC</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Species</t>
+          <t>LYMF</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>WBC</t>
+          <t>RBC</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="H4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>LYMF</t>
+          <t>HGB</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GRAN</t>
+          <t>MCH</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -567,101 +542,58 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
       </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
+      <c r="H6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>MCHC</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="N7" t="n">
+      <c r="H7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RBC</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="n">
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HGB</t>
+          <t>PLT</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>MCH</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>MCHC</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MPV</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>PLT</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+      <c r="D9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: reverted modelFunctions.py to modelCreation_Testing.py
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,11 +457,6 @@
           <t>model4</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -507,9 +502,6 @@
       <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -526,9 +518,6 @@
       <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -548,9 +537,6 @@
       <c r="G6" t="n">
         <v>1</v>
       </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -562,9 +548,6 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: default model trains with all features, including GRAN and MID
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,27 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>newModel</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>newModel2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sdfcsfs</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>adasd</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>model4</t>
+          <t>model2</t>
         </is>
       </c>
     </row>
@@ -487,96 +467,86 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RBC</t>
+          <t>GRAN</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HGB</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MCH</t>
+          <t>RBC</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MCHC</t>
+          <t>HGB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MPV</t>
+          <t>MCH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>MCHC</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MPV</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>PLT</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: prediction by input
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,11 @@
           <t>model2</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>model3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -450,6 +455,9 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -476,6 +484,9 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -497,6 +508,9 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: trained model name is unique
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>defaultModel</t>
+          <t>model5</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -440,6 +440,21 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>model3</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>model7</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>model9</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>model100</t>
         </is>
       </c>
     </row>
@@ -458,6 +473,15 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -471,6 +495,15 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -513,6 +546,9 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -523,6 +559,9 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -533,6 +572,15 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -543,6 +591,15 @@
       <c r="B9" t="n">
         <v>1</v>
       </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -553,6 +610,9 @@
       <c r="B10" t="n">
         <v>1</v>
       </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -561,6 +621,9 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: saving prediction+model implemented for windows os
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,16 @@
           <t>model122</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>yoooo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -463,6 +473,9 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -476,6 +489,9 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -500,6 +516,12 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: saving prediction+model implemented for windows and macos
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,16 @@
           <t>yoooo</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>uhdadhaksd</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dadasds</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -492,6 +502,9 @@
       <c r="E4" t="n">
         <v>1</v>
       </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -505,6 +518,9 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +550,9 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -545,6 +564,9 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: Added about page, detailing model (Hyperlinks don't work atm) ENH: Created about.txt to hold all text for page DEL: Removed all the prediction models that will not be used
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -434,146 +433,274 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>model122</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>test</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>yoooo</t>
+          <t>s</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>uhdadhaksd</t>
+          <t>save</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>dadasds</t>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>test.pkl</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>sa</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>pls</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>revert</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>train</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>save1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>asdfghjkl</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WBC</t>
+          <t>Sex</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LYMF</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GRAN</t>
+          <t>WBC</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LYMF</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RBC</t>
+          <t>GRAN</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HGB</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" t="n">
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MCH</t>
+          <t>RBC</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MCHC</t>
+          <t>HGB</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -583,7 +710,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MPV</t>
+          <t>MCH</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -593,10 +720,30 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>MCHC</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MPV</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>PLT</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: Changed default model to a Random Forest with 66% accuracy ENH: Trained models are now random forests
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -521,6 +521,11 @@
           <t>asdfghjkl</t>
         </is>
       </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>66accuracy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -537,6 +542,9 @@
       <c r="T2" t="n">
         <v>1</v>
       </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -562,6 +570,9 @@
       <c r="T3" t="n">
         <v>1</v>
       </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -599,6 +610,9 @@
       <c r="T4" t="n">
         <v>1</v>
       </c>
+      <c r="U4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -627,6 +641,9 @@
       <c r="T5" t="n">
         <v>1</v>
       </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -658,6 +675,9 @@
       <c r="T6" t="n">
         <v>1</v>
       </c>
+      <c r="U6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -680,6 +700,9 @@
       <c r="T7" t="n">
         <v>1</v>
       </c>
+      <c r="U7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -696,6 +719,9 @@
       <c r="M8" t="n">
         <v>1</v>
       </c>
+      <c r="U8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -706,6 +732,9 @@
       <c r="B9" t="n">
         <v>1</v>
       </c>
+      <c r="U9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -716,6 +745,9 @@
       <c r="B10" t="n">
         <v>1</v>
       </c>
+      <c r="U10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -724,6 +756,9 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: Replaced default model with one that uses all features
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -526,6 +526,21 @@
           <t>66accuracy</t>
         </is>
       </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>trainedModel</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>testing3</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>PLT</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -545,6 +560,9 @@
       <c r="U2" t="n">
         <v>1</v>
       </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -573,6 +591,9 @@
       <c r="U3" t="n">
         <v>1</v>
       </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -613,6 +634,9 @@
       <c r="U4" t="n">
         <v>1</v>
       </c>
+      <c r="V4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -644,6 +668,9 @@
       <c r="U5" t="n">
         <v>1</v>
       </c>
+      <c r="V5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -678,6 +705,9 @@
       <c r="U6" t="n">
         <v>1</v>
       </c>
+      <c r="V6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -703,6 +733,12 @@
       <c r="U7" t="n">
         <v>1</v>
       </c>
+      <c r="V7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -722,6 +758,9 @@
       <c r="U8" t="n">
         <v>1</v>
       </c>
+      <c r="V8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -735,6 +774,9 @@
       <c r="U9" t="n">
         <v>1</v>
       </c>
+      <c r="V9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -748,6 +790,9 @@
       <c r="U10" t="n">
         <v>1</v>
       </c>
+      <c r="V10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -759,6 +804,12 @@
         <v>1</v>
       </c>
       <c r="U11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" t="n">
+        <v>1</v>
+      </c>
+      <c r="X11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: reverted to decision tree and re-added about page
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
           <t>dadasds</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>save5</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -470,6 +475,9 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +494,9 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -505,6 +516,9 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -519,6 +533,9 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: loading a model works properly
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,10 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -433,403 +434,145 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>model3</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>help</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>help</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>test.pkl</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>save</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>sa</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>pls</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>revert</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>train</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>save1</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>asdfghjkl</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>66accuracy</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>trainedModel</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>testing3</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>PLT</t>
+          <t>model5</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>WBC</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" t="n">
+      <c r="C2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Species</t>
+          <t>LYMF</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" t="n">
+      <c r="C3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>WBC</t>
+          <t>GRAN</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
       <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>LYMF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
       <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GRAN</t>
+          <t>RBC</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" t="n">
-        <v>1</v>
-      </c>
-      <c r="U6" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" t="n">
+      <c r="C6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>HGB</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" t="n">
-        <v>1</v>
-      </c>
-      <c r="U7" t="n">
-        <v>1</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1</v>
-      </c>
-      <c r="W7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RBC</t>
+          <t>MCH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="U8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HGB</t>
+          <t>MCHC</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
-      <c r="U9" t="n">
-        <v>1</v>
-      </c>
-      <c r="V9" t="n">
+      <c r="D9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MCH</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
-      <c r="U10" t="n">
-        <v>1</v>
-      </c>
-      <c r="V10" t="n">
+      <c r="D10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MCHC</t>
+          <t>PLT</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
-      <c r="U11" t="n">
-        <v>1</v>
-      </c>
-      <c r="V11" t="n">
-        <v>1</v>
-      </c>
-      <c r="X11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MPV</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>PLT</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+      <c r="D11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROD: save the result when inputting the value manually
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,31 @@
           <t>defaultModel</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>newModel</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>newModel2</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>newModel3</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>newModel7</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>newModel1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -442,6 +467,21 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -482,6 +522,21 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -502,6 +557,21 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -520,6 +590,21 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUG: saving prediction when import + added a new text field for seal tag when inputing
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
           <t>newModel1</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>modelmodel1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,6 +487,9 @@
       <c r="G2" t="n">
         <v>1</v>
       </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -492,6 +500,9 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -500,6 +511,9 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROD: Species removed when training and predicting
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,11 @@
           <t>modelmodel1</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -490,6 +495,9 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -503,6 +511,9 @@
       <c r="H3" t="n">
         <v>1</v>
       </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +525,9 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROD: removed species input text field from prediction window
</commit_message>
<xml_diff>
--- a/GUI/featuresChecklist.xlsx
+++ b/GUI/featuresChecklist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,41 +432,6 @@
           <t>defaultModel</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>newModel</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>newModel2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>newModel3</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>newModel7</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>newModel1</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>modelmodel1</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -477,27 +442,6 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -508,12 +452,6 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -524,12 +462,6 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -550,21 +482,6 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -585,21 +502,6 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -618,21 +520,6 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>